<commit_message>
update clothes.xlsx, food.xlsx, material.xlsx, products.xlsx and tables.sql, add .gitignore
</commit_message>
<xml_diff>
--- a/Excel/clothes.xlsx
+++ b/Excel/clothes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utilisateur\Documents\BD6\projet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hugo/Desktop/school-uni-bd6/Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E2028451-90E2-437A-AF2E-EF77E6AEEED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93597BFA-F25B-C943-AEDF-D96756F14D01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3075" yWindow="3075" windowWidth="21600" windowHeight="11385" xr2:uid="{BB886CCD-29D6-4CD6-A752-F6470C720E79}"/>
+    <workbookView xWindow="3100" yWindow="1860" windowWidth="21600" windowHeight="11380" xr2:uid="{BB886CCD-29D6-4CD6-A752-F6470C720E79}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>product_id</t>
   </si>
@@ -47,6 +47,21 @@
   </si>
   <si>
     <t>unit_weight</t>
+  </si>
+  <si>
+    <t>Chanvre</t>
+  </si>
+  <si>
+    <t>Fourrure</t>
+  </si>
+  <si>
+    <t>Cuir</t>
+  </si>
+  <si>
+    <t>Argent</t>
+  </si>
+  <si>
+    <t>Or</t>
   </si>
 </sst>
 </file>
@@ -398,15 +413,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A32CA59-5659-4968-84F3-153F2C55A849}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -418,6 +433,76 @@
       </c>
       <c r="D1" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>38</v>
+      </c>
+      <c r="D3">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>6</v>
+      </c>
+      <c r="D4">
+        <v>0.32100000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>54</v>
+      </c>
+      <c r="D5">
+        <v>0.152</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>102</v>
+      </c>
+      <c r="D6">
+        <v>0.20200000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add CSV and the first psql request
</commit_message>
<xml_diff>
--- a/Excel/clothes.xlsx
+++ b/Excel/clothes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hugo/Desktop/school-uni-bd6/Excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utilisateur\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93597BFA-F25B-C943-AEDF-D96756F14D01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F374C8D3-31FB-4FC3-B59F-E43001FD1695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3100" yWindow="1860" windowWidth="21600" windowHeight="11380" xr2:uid="{BB886CCD-29D6-4CD6-A752-F6470C720E79}"/>
+    <workbookView xWindow="3675" yWindow="3675" windowWidth="21600" windowHeight="11385" xr2:uid="{BB886CCD-29D6-4CD6-A752-F6470C720E79}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>product_id</t>
   </si>
@@ -62,6 +62,21 @@
   </si>
   <si>
     <t>Or</t>
+  </si>
+  <si>
+    <t>0.45</t>
+  </si>
+  <si>
+    <t>2.2</t>
+  </si>
+  <si>
+    <t>0.321</t>
+  </si>
+  <si>
+    <t>0.152</t>
+  </si>
+  <si>
+    <t>0.202</t>
   </si>
 </sst>
 </file>
@@ -416,12 +431,12 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -435,7 +450,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>4</v>
       </c>
@@ -445,11 +460,11 @@
       <c r="C2">
         <v>2</v>
       </c>
-      <c r="D2">
-        <v>0.45</v>
+      <c r="D2" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>17</v>
       </c>
@@ -459,11 +474,11 @@
       <c r="C3">
         <v>38</v>
       </c>
-      <c r="D3">
-        <v>2.2000000000000002</v>
+      <c r="D3" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>18</v>
       </c>
@@ -473,11 +488,11 @@
       <c r="C4">
         <v>6</v>
       </c>
-      <c r="D4">
-        <v>0.32100000000000001</v>
+      <c r="D4" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>19</v>
       </c>
@@ -487,11 +502,11 @@
       <c r="C5">
         <v>54</v>
       </c>
-      <c r="D5">
-        <v>0.152</v>
+      <c r="D5" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>25</v>
       </c>
@@ -501,8 +516,8 @@
       <c r="C6">
         <v>102</v>
       </c>
-      <c r="D6">
-        <v>0.20200000000000001</v>
+      <c r="D6" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>